<commit_message>
Added testing for moving other formats correctly.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/AllConditionalFormatting.xlsx
+++ b/EPPlusTest/Workbooks/AllConditionalFormatting.xlsx
@@ -305,13 +305,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF002060"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFFFFF00"/>
       </font>
@@ -374,6 +367,13 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
         </patternFill>
       </fill>
     </dxf>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="M73" sqref="M73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,22 +1822,22 @@
     <cfRule type="top10" dxfId="28" priority="9" bottom="1" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39:I50">
-    <cfRule type="top10" dxfId="18" priority="8" percent="1" bottom="1" rank="20"/>
+    <cfRule type="top10" dxfId="27" priority="8" percent="1" bottom="1" rank="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C66">
-    <cfRule type="aboveAverage" dxfId="27" priority="7"/>
+    <cfRule type="aboveAverage" dxfId="26" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:E66">
-    <cfRule type="aboveAverage" dxfId="26" priority="6" equalAverage="1"/>
+    <cfRule type="aboveAverage" dxfId="25" priority="6" equalAverage="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G55:G66">
-    <cfRule type="aboveAverage" dxfId="25" priority="5" aboveAverage="0" stdDev="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C71:C83 C86">
-    <cfRule type="duplicateValues" dxfId="24" priority="4"/>
+    <cfRule type="aboveAverage" dxfId="24" priority="5" aboveAverage="0" stdDev="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71:C83">
+    <cfRule type="duplicateValues" dxfId="23" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E71:E83">
-    <cfRule type="uniqueValues" dxfId="23" priority="3"/>
+    <cfRule type="uniqueValues" dxfId="22" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:I16">
     <cfRule type="iconSet" priority="32">
@@ -1851,18 +1851,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C33">
-    <cfRule type="cellIs" dxfId="22" priority="33" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="33" operator="between">
       <formula>$Q$22</formula>
       <formula>$Q$23</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87">
-    <cfRule type="expression" dxfId="21" priority="34">
+    <cfRule type="expression" dxfId="20" priority="34">
       <formula>TODAY()/1000&gt;$E$87</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88">
-    <cfRule type="expression" dxfId="20" priority="35">
+    <cfRule type="expression" dxfId="19" priority="35">
       <formula>TODAY()/1000&lt;$E$87</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated conditional formatting with space seperated addresses to select and work correctly.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/AllConditionalFormatting.xlsx
+++ b/EPPlusTest/Workbooks/AllConditionalFormatting.xlsx
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="M73" sqref="M73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,12 +754,12 @@
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -773,7 +773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>1</v>
       </c>
@@ -787,7 +787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>2</v>
       </c>
@@ -812,8 +812,11 @@
       <c r="Q6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="S6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>3</v>
       </c>
@@ -832,8 +835,11 @@
       <c r="Q7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="S7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>4</v>
       </c>
@@ -849,8 +855,11 @@
       <c r="Q8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="S8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>5</v>
       </c>
@@ -867,7 +876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>6</v>
       </c>
@@ -884,7 +893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>7</v>
       </c>
@@ -898,7 +907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>8</v>
       </c>
@@ -912,7 +921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>9</v>
       </c>
@@ -926,7 +935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>10</v>
       </c>
@@ -940,7 +949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>11</v>
       </c>
@@ -954,7 +963,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>12</v>
       </c>
@@ -1005,7 +1014,7 @@
       </c>
       <c r="G22" s="1">
         <f ca="1">TODAY()</f>
-        <v>43095</v>
+        <v>43109</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -1035,7 +1044,7 @@
       </c>
       <c r="G23" s="1">
         <f ca="1">TODAY()-3</f>
-        <v>43092</v>
+        <v>43106</v>
       </c>
       <c r="I23">
         <v>2</v>
@@ -1062,7 +1071,7 @@
       </c>
       <c r="G24" s="1">
         <f ca="1">TODAY()-5</f>
-        <v>43090</v>
+        <v>43104</v>
       </c>
       <c r="I24">
         <v>3</v>
@@ -1086,7 +1095,7 @@
       </c>
       <c r="G25" s="1">
         <f t="shared" ref="G25" ca="1" si="0">TODAY()-3</f>
-        <v>43092</v>
+        <v>43106</v>
       </c>
       <c r="M25" t="e">
         <f ca="1">BLAH()</f>
@@ -1106,7 +1115,7 @@
       </c>
       <c r="G26" s="1">
         <f ca="1">TODAY()-6</f>
-        <v>43089</v>
+        <v>43103</v>
       </c>
       <c r="M26">
         <v>5</v>
@@ -1124,7 +1133,7 @@
       </c>
       <c r="G27" s="1">
         <f ca="1">TODAY()-7</f>
-        <v>43088</v>
+        <v>43102</v>
       </c>
       <c r="I27">
         <v>6</v>
@@ -1150,7 +1159,7 @@
       </c>
       <c r="G28" s="1">
         <f ca="1">TODAY()-8</f>
-        <v>43087</v>
+        <v>43101</v>
       </c>
       <c r="I28">
         <v>7</v>
@@ -1174,7 +1183,7 @@
       </c>
       <c r="G29" s="1">
         <f ca="1">TODAY()-9</f>
-        <v>43086</v>
+        <v>43100</v>
       </c>
       <c r="I29" t="str">
         <f>""</f>
@@ -1214,7 +1223,7 @@
       </c>
       <c r="G31" s="1">
         <f ca="1">TODAY()-100</f>
-        <v>42995</v>
+        <v>43009</v>
       </c>
       <c r="I31">
         <v>10</v>
@@ -1238,7 +1247,7 @@
       </c>
       <c r="G32" s="1">
         <f ca="1">TODAY()-1000</f>
-        <v>42095</v>
+        <v>42109</v>
       </c>
       <c r="I32">
         <v>11</v>
@@ -1262,7 +1271,7 @@
       </c>
       <c r="G33" s="1">
         <f ca="1">TODAY()-100</f>
-        <v>42995</v>
+        <v>43009</v>
       </c>
       <c r="I33" t="str">
         <f>""</f>
@@ -1773,7 +1782,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G16">
+  <conditionalFormatting sqref="G5:G16 S6:S8">
     <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="min"/>
@@ -1882,7 +1891,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G5:G16</xm:sqref>
+          <xm:sqref>G5:G16 S6:S8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="18" operator="containsText" id="{19E03278-CF34-4ED7-96AB-CCB567C35F4E}">

</xml_diff>